<commit_message>
Power output calculation corrected
</commit_message>
<xml_diff>
--- a/TrainerPower.xlsx
+++ b/TrainerPower.xlsx
@@ -29,7 +29,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -53,6 +53,12 @@
     </font>
     <font>
       <sz val="18"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
@@ -83,7 +89,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -130,6 +136,37 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="11"/>
       </left>
       <right style="thin">
@@ -141,6 +178,31 @@
       <bottom style="thin">
         <color indexed="13"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -274,22 +336,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="10"/>
       </left>
@@ -326,7 +372,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -342,52 +388,52 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -397,6 +443,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -424,6 +482,7 @@
       <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ff878787"/>
       <rgbColor rgb="ff009ef9"/>
+      <rgbColor rgb="ff33b4ff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -434,6 +493,48 @@
   <c:date1904 val="0"/>
   <c:roundedCorners val="0"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" i="0" strike="noStrike" sz="1800" u="none">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Helvetica Neue"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" i="0" strike="noStrike" sz="1800" u="none">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Helvetica Neue"/>
+              </a:rPr>
+              <a:t>Speed-Power Curve</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.311086"/>
+          <c:y val="0"/>
+          <c:w val="0.377828"/>
+          <c:h val="0.121536"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout>
@@ -441,37 +542,35 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.123772"/>
-          <c:y val="0.0716533"/>
-          <c:w val="0.870603"/>
-          <c:h val="0.877564"/>
+          <c:x val="0.189136"/>
+          <c:y val="0.121536"/>
+          <c:w val="0.786554"/>
+          <c:h val="0.681578"/>
         </c:manualLayout>
       </c:layout>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Power</c:v>
+            <c:v>Speed-Power Kurve</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln w="47625" cap="flat">
-              <a:solidFill>
-                <a:srgbClr val="009EF9"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="9"/>
+            <c:symbol val="plus"/>
+            <c:size val="10"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -511,102 +610,252 @@
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="11"/>
-              <c:pt idx="0">
-                <c:v>Ohne Titel 1</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>Ohne Titel 2</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>Ohne Titel 3</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>Ohne Titel 4</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>Ohne Titel 5</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>Ohne Titel 6</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>Ohne Titel 7</c:v>
-              </c:pt>
-              <c:pt idx="7">
-                <c:v>Ohne Titel 8</c:v>
-              </c:pt>
-              <c:pt idx="8">
-                <c:v>Ohne Titel 9</c:v>
-              </c:pt>
-              <c:pt idx="9">
-                <c:v>Ohne Titel 10</c:v>
-              </c:pt>
-              <c:pt idx="10">
-                <c:v>Ohne Titel 11</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
-          <c:val>
+          <c:trendline>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="25400" cap="flat">
+                <a:solidFill>
+                  <a:srgbClr val="33B4FF"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:miter lim="400000"/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="tl" rotWithShape="1" blurRad="12700" dist="25400" dir="7320000">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="25000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr b="0" i="0" strike="noStrike" sz="1000" u="none">
+                        <a:solidFill>
+                          <a:srgbClr val="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Helvetica Neue"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr b="0" i="0" strike="noStrike" sz="1000" u="none">
+                        <a:solidFill>
+                          <a:srgbClr val="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Helvetica Neue"/>
+                      </a:rPr>
+                      <a:t>y = -0,0009x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr b="0" baseline="33200" i="0" strike="noStrike" sz="1000" u="none">
+                        <a:solidFill>
+                          <a:srgbClr val="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Helvetica Neue"/>
+                      </a:rPr>
+                      <a:t>3</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr b="0" i="0" strike="noStrike" sz="1000" u="none">
+                        <a:solidFill>
+                          <a:srgbClr val="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Helvetica Neue"/>
+                      </a:rPr>
+                      <a:t> + 0,1173x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr b="0" baseline="33200" i="0" strike="noStrike" sz="1000" u="none">
+                        <a:solidFill>
+                          <a:srgbClr val="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Helvetica Neue"/>
+                      </a:rPr>
+                      <a:t>2</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr b="0" i="0" strike="noStrike" sz="1000" u="none">
+                        <a:solidFill>
+                          <a:srgbClr val="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Helvetica Neue"/>
+                      </a:rPr>
+                      <a:t> + 3,437x - 1,236</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
             <c:numRef>
-              <c:f>'Blatt 1 - Elite Novo Force Mag '!$B$3:$B$13</c:f>
+              <c:f>'Blatt 1 - Elite Novo Force Mag '!$A$2:$A$16</c:f>
               <c:numCache>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0.000010</c:v>
-                </c:pt>
+                <c:ptCount val="14"/>
                 <c:pt idx="1">
-                  <c:v>25.000000</c:v>
+                  <c:v>0.000000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60.000000</c:v>
+                  <c:v>10.000000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>85.000000</c:v>
+                  <c:v>16.000000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>120.000000</c:v>
+                  <c:v>18.000000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>150.000000</c:v>
+                  <c:v>21.500000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>180.000000</c:v>
+                  <c:v>24.500000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>220.000000</c:v>
+                  <c:v>26.000000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>260.000000</c:v>
+                  <c:v>29.000000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>300.000000</c:v>
+                  <c:v>32.000000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>345.000000</c:v>
+                  <c:v>34.000000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>37.000000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40.000000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>45.000000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>48.000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Blatt 1 - Elite Novo Force Mag '!$B$2:$B$16</c:f>
+              <c:numCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="1">
+                  <c:v>0.000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40.000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80.000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>95.000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>120.000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>140.000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>154.000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>176.000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>200.000000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>216.000000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>241.000000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>266.000000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>311.000000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>338.000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:marker val="1"/>
         <c:axId val="2094734552"/>
         <c:axId val="2094734553"/>
-      </c:lineChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="2094734552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="55"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="12700" cap="flat">
+              <a:solidFill>
+                <a:srgbClr val="888888"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" i="0" strike="noStrike" sz="1800" u="none">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Helvetica Neue"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" i="0" strike="noStrike" sz="1800" u="none">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Helvetica Neue"/>
+                  </a:rPr>
+                  <a:t>Speed in kmH</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="1"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="none"/>
+        <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln w="12700" cap="flat">
             <a:solidFill>
@@ -632,14 +881,16 @@
         </c:txPr>
         <c:crossAx val="2094734553"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:noMultiLvlLbl val="1"/>
-      </c:catAx>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="13.75"/>
+        <c:minorUnit val="6.875"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="2094734553"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="400"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -654,6 +905,35 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" i="0" strike="noStrike" sz="1800" u="none">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Helvetica Neue"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" i="0" strike="noStrike" sz="1800" u="none">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Helvetica Neue"/>
+                  </a:rPr>
+                  <a:t>Power in Watts</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="1"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -683,7 +963,7 @@
         </c:txPr>
         <c:crossAx val="2094734552"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
         <c:majorUnit val="100"/>
         <c:minorUnit val="50"/>
       </c:valAx>
@@ -721,25 +1001,25 @@
 <xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>109270</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>736600</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>143510</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>511098</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>52628</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="2D-Liniendiagramm"/>
+        <xdr:cNvPr id="2" name="Streudiagramm"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9347200" y="0"/>
-        <a:ext cx="5080000" cy="3810000"/>
+        <a:off x="-409499" y="13041045"/>
+        <a:ext cx="5489499" cy="4492499"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1778,14 +2058,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="7" width="16.3516" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="12" width="16.3516" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
@@ -1798,576 +2078,883 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="4"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="7"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="5">
+      <c r="A2" t="s" s="8">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="5">
+      <c r="B2" t="s" s="8">
         <v>2</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="12"/>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" s="7">
+      <c r="A3" s="13">
         <v>0</v>
       </c>
-      <c r="B3" s="8">
-        <v>1e-05</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="B3" s="14">
+        <v>0</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="12"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="10">
-        <v>5</v>
-      </c>
-      <c r="B4" s="11">
-        <v>25</v>
-      </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
+      <c r="A4" s="16">
+        <v>10</v>
+      </c>
+      <c r="B4" s="17">
+        <v>40</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="12"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="10">
-        <v>10</v>
-      </c>
-      <c r="B5" s="11">
-        <v>60</v>
-      </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
+      <c r="A5" s="16">
+        <v>16</v>
+      </c>
+      <c r="B5" s="17">
+        <v>80</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="12"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="10">
-        <v>15</v>
-      </c>
-      <c r="B6" s="11">
-        <v>85</v>
-      </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
+      <c r="A6" s="16">
+        <v>18</v>
+      </c>
+      <c r="B6" s="17">
+        <v>95</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="12"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="10">
-        <v>20</v>
-      </c>
-      <c r="B7" s="11">
+      <c r="A7" s="16">
+        <v>21.5</v>
+      </c>
+      <c r="B7" s="17">
         <v>120</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="12"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="10">
-        <v>25</v>
-      </c>
-      <c r="B8" s="11">
-        <v>150</v>
-      </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
+      <c r="A8" s="16">
+        <v>24.5</v>
+      </c>
+      <c r="B8" s="17">
+        <v>140</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="12"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="10">
-        <v>30</v>
-      </c>
-      <c r="B9" s="11">
-        <v>180</v>
-      </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
+      <c r="A9" s="16">
+        <v>26</v>
+      </c>
+      <c r="B9" s="17">
+        <v>154</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="12"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="10">
-        <v>35</v>
-      </c>
-      <c r="B10" s="11">
-        <v>220</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
+      <c r="A10" s="16">
+        <v>29</v>
+      </c>
+      <c r="B10" s="17">
+        <v>176</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="12"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="10">
+      <c r="A11" s="16">
+        <v>32</v>
+      </c>
+      <c r="B11" s="17">
+        <v>200</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="12"/>
+    </row>
+    <row r="12" ht="20.05" customHeight="1">
+      <c r="A12" s="16">
+        <v>34</v>
+      </c>
+      <c r="B12" s="17">
+        <v>216</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="12"/>
+    </row>
+    <row r="13" ht="20.05" customHeight="1">
+      <c r="A13" s="16">
+        <v>37</v>
+      </c>
+      <c r="B13" s="17">
+        <v>241</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="12"/>
+    </row>
+    <row r="14" ht="20.05" customHeight="1">
+      <c r="A14" s="16">
         <v>40</v>
       </c>
-      <c r="B11" s="11">
-        <v>260</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-    </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="10">
+      <c r="B14" s="17">
+        <v>266</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="12"/>
+    </row>
+    <row r="15" ht="20.05" customHeight="1">
+      <c r="A15" s="16">
         <v>45</v>
       </c>
-      <c r="B12" s="11">
-        <v>300</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-    </row>
-    <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="10">
-        <v>50</v>
-      </c>
-      <c r="B13" s="11">
-        <v>345</v>
-      </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-    </row>
-    <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-    </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
+      <c r="B15" s="17">
+        <v>311</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="12"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="13"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
+      <c r="A16" s="16">
+        <v>48</v>
+      </c>
+      <c r="B16" s="17">
+        <v>338</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="12"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="13"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="12"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="13"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="12"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="12"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="13"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="12"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="12"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="13"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="12"/>
     </row>
     <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="13"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="12"/>
     </row>
     <row r="24" ht="14.7" customHeight="1">
-      <c r="A24" s="15"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="17"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="12"/>
     </row>
     <row r="25" ht="14.7" customHeight="1">
-      <c r="A25" s="18"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="20"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="12"/>
     </row>
     <row r="26" ht="14.7" customHeight="1">
-      <c r="A26" s="18"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="20"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="12"/>
     </row>
     <row r="27" ht="14.7" customHeight="1">
-      <c r="A27" s="18"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="20"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="12"/>
     </row>
     <row r="28" ht="14.7" customHeight="1">
-      <c r="A28" s="18"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="20"/>
+      <c r="A28" s="24"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="12"/>
     </row>
     <row r="29" ht="14.7" customHeight="1">
-      <c r="A29" s="18"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="20"/>
+      <c r="A29" s="24"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="12"/>
     </row>
     <row r="30" ht="14.7" customHeight="1">
-      <c r="A30" s="18"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="20"/>
+      <c r="A30" s="24"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="12"/>
     </row>
     <row r="31" ht="14.7" customHeight="1">
-      <c r="A31" s="18"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="20"/>
+      <c r="A31" s="24"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="12"/>
     </row>
     <row r="32" ht="14.7" customHeight="1">
-      <c r="A32" s="18"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="20"/>
+      <c r="A32" s="24"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="12"/>
     </row>
     <row r="33" ht="14.7" customHeight="1">
-      <c r="A33" s="18"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="20"/>
+      <c r="A33" s="24"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="12"/>
     </row>
     <row r="34" ht="14.7" customHeight="1">
-      <c r="A34" s="18"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="20"/>
+      <c r="A34" s="24"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="12"/>
     </row>
     <row r="35" ht="14.7" customHeight="1">
-      <c r="A35" s="18"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="20"/>
+      <c r="A35" s="24"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="12"/>
     </row>
     <row r="36" ht="14.7" customHeight="1">
-      <c r="A36" s="18"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="20"/>
+      <c r="A36" s="24"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="12"/>
     </row>
     <row r="37" ht="14.7" customHeight="1">
-      <c r="A37" s="18"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="20"/>
+      <c r="A37" s="24"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="12"/>
     </row>
     <row r="38" ht="14.7" customHeight="1">
-      <c r="A38" s="18"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="20"/>
+      <c r="A38" s="24"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="12"/>
     </row>
     <row r="39" ht="14.7" customHeight="1">
-      <c r="A39" s="18"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="20"/>
+      <c r="A39" s="24"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="12"/>
     </row>
     <row r="40" ht="14.7" customHeight="1">
-      <c r="A40" s="18"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="20"/>
+      <c r="A40" s="24"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="12"/>
     </row>
     <row r="41" ht="14.7" customHeight="1">
-      <c r="A41" s="18"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="20"/>
+      <c r="A41" s="24"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="12"/>
     </row>
     <row r="42" ht="14.7" customHeight="1">
-      <c r="A42" s="18"/>
-      <c r="B42" s="19"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="20"/>
+      <c r="A42" s="24"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="12"/>
     </row>
     <row r="43" ht="14.7" customHeight="1">
-      <c r="A43" s="18"/>
-      <c r="B43" s="19"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="20"/>
+      <c r="A43" s="24"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="12"/>
     </row>
     <row r="44" ht="14.7" customHeight="1">
-      <c r="A44" s="18"/>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="19"/>
-      <c r="G44" s="20"/>
+      <c r="A44" s="24"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="12"/>
     </row>
     <row r="45" ht="14.7" customHeight="1">
-      <c r="A45" s="18"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="20"/>
+      <c r="A45" s="24"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="12"/>
     </row>
     <row r="46" ht="14.7" customHeight="1">
-      <c r="A46" s="18"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="20"/>
+      <c r="A46" s="24"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="24"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11"/>
+      <c r="K46" s="11"/>
+      <c r="L46" s="12"/>
     </row>
     <row r="47" ht="14.7" customHeight="1">
-      <c r="A47" s="18"/>
-      <c r="B47" s="19"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="19"/>
-      <c r="G47" s="20"/>
+      <c r="A47" s="24"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="24"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="12"/>
     </row>
     <row r="48" ht="14.7" customHeight="1">
-      <c r="A48" s="18"/>
-      <c r="B48" s="19"/>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="20"/>
+      <c r="A48" s="24"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="12"/>
     </row>
     <row r="49" ht="14.7" customHeight="1">
-      <c r="A49" s="18"/>
-      <c r="B49" s="19"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="20"/>
+      <c r="A49" s="24"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="24"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="11"/>
+      <c r="K49" s="11"/>
+      <c r="L49" s="12"/>
     </row>
     <row r="50" ht="14.7" customHeight="1">
-      <c r="A50" s="18"/>
-      <c r="B50" s="19"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="20"/>
+      <c r="A50" s="24"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="24"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="11"/>
+      <c r="L50" s="12"/>
     </row>
     <row r="51" ht="14.7" customHeight="1">
-      <c r="A51" s="18"/>
-      <c r="B51" s="19"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="20"/>
+      <c r="A51" s="24"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="12"/>
+      <c r="H51" s="24"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="11"/>
+      <c r="L51" s="12"/>
     </row>
     <row r="52" ht="14.7" customHeight="1">
-      <c r="A52" s="18"/>
-      <c r="B52" s="19"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="20"/>
+      <c r="A52" s="24"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="12"/>
+      <c r="H52" s="24"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="11"/>
+      <c r="K52" s="11"/>
+      <c r="L52" s="12"/>
     </row>
     <row r="53" ht="14.7" customHeight="1">
-      <c r="A53" s="18"/>
-      <c r="B53" s="19"/>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="20"/>
+      <c r="A53" s="24"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="24"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="11"/>
+      <c r="K53" s="11"/>
+      <c r="L53" s="12"/>
     </row>
     <row r="54" ht="14.7" customHeight="1">
-      <c r="A54" s="18"/>
-      <c r="B54" s="19"/>
-      <c r="C54" s="19"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="19"/>
-      <c r="F54" s="19"/>
-      <c r="G54" s="20"/>
+      <c r="A54" s="24"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="24"/>
+      <c r="I54" s="11"/>
+      <c r="J54" s="11"/>
+      <c r="K54" s="11"/>
+      <c r="L54" s="12"/>
     </row>
     <row r="55" ht="14.7" customHeight="1">
-      <c r="A55" s="18"/>
-      <c r="B55" s="19"/>
-      <c r="C55" s="19"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="19"/>
-      <c r="G55" s="20"/>
+      <c r="A55" s="24"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="24"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="11"/>
+      <c r="K55" s="11"/>
+      <c r="L55" s="12"/>
     </row>
     <row r="56" ht="14.7" customHeight="1">
-      <c r="A56" s="18"/>
-      <c r="B56" s="19"/>
-      <c r="C56" s="19"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="19"/>
-      <c r="G56" s="20"/>
+      <c r="A56" s="24"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="24"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="11"/>
+      <c r="L56" s="12"/>
     </row>
     <row r="57" ht="14.7" customHeight="1">
-      <c r="A57" s="18"/>
-      <c r="B57" s="19"/>
-      <c r="C57" s="19"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="19"/>
-      <c r="G57" s="20"/>
+      <c r="A57" s="24"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="24"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="11"/>
+      <c r="K57" s="11"/>
+      <c r="L57" s="12"/>
     </row>
     <row r="58" ht="14.7" customHeight="1">
-      <c r="A58" s="18"/>
-      <c r="B58" s="19"/>
-      <c r="C58" s="19"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="19"/>
-      <c r="F58" s="19"/>
-      <c r="G58" s="20"/>
+      <c r="A58" s="24"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="24"/>
+      <c r="I58" s="11"/>
+      <c r="J58" s="11"/>
+      <c r="K58" s="11"/>
+      <c r="L58" s="12"/>
     </row>
     <row r="59" ht="14.7" customHeight="1">
-      <c r="A59" s="21"/>
-      <c r="B59" s="22"/>
-      <c r="C59" s="22"/>
-      <c r="D59" s="22"/>
-      <c r="E59" s="22"/>
-      <c r="F59" s="22"/>
-      <c r="G59" s="23"/>
+      <c r="A59" s="25"/>
+      <c r="B59" s="26"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="26"/>
+      <c r="E59" s="26"/>
+      <c r="F59" s="26"/>
+      <c r="G59" s="27"/>
+      <c r="H59" s="25"/>
+      <c r="I59" s="26"/>
+      <c r="J59" s="26"/>
+      <c r="K59" s="26"/>
+      <c r="L59" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>